<commit_message>
update nvprof result of all benchmarks
</commit_message>
<xml_diff>
--- a/Nvprof summary/MM-Similarity.xlsx
+++ b/Nvprof summary/MM-Similarity.xlsx
@@ -5,18 +5,18 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyc/Documents/Github/GPU-DATA-PLACEMENT/MM/prof/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyc/Documents/Github/GPU-DATA-PLACEMENT/Nvprof summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="460" windowWidth="25520" windowHeight="15540"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
+    <sheet name="Ref1" sheetId="5" r:id="rId4"/>
+    <sheet name="Ref2" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="896">
   <si>
     <t>Event Name</t>
   </si>
@@ -2713,6 +2713,9 @@
   </si>
   <si>
     <t>Ref1</t>
+  </si>
+  <si>
+    <t>Performance</t>
   </si>
 </sst>
 </file>
@@ -3107,7 +3110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+    <sheetView topLeftCell="A115" workbookViewId="0">
       <selection activeCell="A84" sqref="A84:XFD84"/>
     </sheetView>
   </sheetViews>
@@ -19881,7 +19884,7 @@
         <v>43.06449109676241</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O2:O33" si="12">B3/$N3</f>
+        <f t="shared" ref="O3:O33" si="12">B3/$N3</f>
         <v>0</v>
       </c>
       <c r="P3">
@@ -20023,7 +20026,7 @@
         <v>0</v>
       </c>
       <c r="Z4" s="6">
-        <f t="shared" ref="Z2:AA33" si="14">(O4-$O$78)^2+(P4-$P$78)^2+(Q4-$Q$78)^2+(R4-$R$78)^2+(S4-$S$78)^2+(T4-$T$78)^2+(U4-$U$78)^2+(V4-$V$78)^2+(W4-$W$78)^2+(X4-$X$78)^2+(Y4-$Y$78)^2</f>
+        <f t="shared" ref="Z4:Z33" si="14">(O4-$O$78)^2+(P4-$P$78)^2+(Q4-$Q$78)^2+(R4-$R$78)^2+(S4-$S$78)^2+(T4-$T$78)^2+(U4-$U$78)^2+(V4-$V$78)^2+(W4-$W$78)^2+(X4-$X$78)^2+(Y4-$Y$78)^2</f>
         <v>1.7026276120426931</v>
       </c>
       <c r="AA4">
@@ -26047,7 +26050,7 @@
         <v>619</v>
       </c>
       <c r="M66">
-        <f t="shared" ref="M66:M79" si="29">$B66*$B66+$C66*$C66+$D66*$D66+$E66*$E66+$F66*$F66+$G66*$G66+$H66*$H66+$I66*$I66+$J66*$J66+$K66*$K66+$L66*$L66</f>
+        <f t="shared" ref="M66:M78" si="29">$B66*$B66+$C66*$C66+$D66*$D66+$E66*$E66+$F66*$F66+$G66*$G66+$H66*$H66+$I66*$I66+$J66*$J66+$K66*$K66+$L66*$L66</f>
         <v>163296073043581</v>
       </c>
       <c r="N66" s="5">
@@ -26055,51 +26058,51 @@
         <v>12778735.189508429</v>
       </c>
       <c r="O66">
-        <f t="shared" ref="O66:O79" si="31">B66/$N66</f>
+        <f t="shared" ref="O66:O78" si="31">B66/$N66</f>
         <v>0.23235241641424279</v>
       </c>
       <c r="P66">
-        <f t="shared" ref="P66:P79" si="32">C66/$N66</f>
+        <f t="shared" ref="P66:P78" si="32">C66/$N66</f>
         <v>0.17684794046404631</v>
       </c>
       <c r="Q66">
-        <f t="shared" ref="Q66:Q79" si="33">D66/$N66</f>
+        <f t="shared" ref="Q66:Q78" si="33">D66/$N66</f>
         <v>0.17682469872723938</v>
       </c>
       <c r="R66">
-        <f t="shared" ref="R66:R79" si="34">E66/$N66</f>
+        <f t="shared" ref="R66:R78" si="34">E66/$N66</f>
         <v>0.77272013650514082</v>
       </c>
       <c r="S66">
-        <f t="shared" ref="S66:S79" si="35">F66/$N66</f>
+        <f t="shared" ref="S66:S78" si="35">F66/$N66</f>
         <v>0.23126021129432928</v>
       </c>
       <c r="T66">
-        <f t="shared" ref="T66:T79" si="36">G66/$N66</f>
+        <f t="shared" ref="T66:T78" si="36">G66/$N66</f>
         <v>0.17178437204037908</v>
       </c>
       <c r="U66">
-        <f t="shared" ref="U66:U79" si="37">H66/$N66</f>
+        <f t="shared" ref="U66:U78" si="37">H66/$N66</f>
         <v>0.17218010760614555</v>
       </c>
       <c r="V66">
-        <f t="shared" ref="V66:V79" si="38">I66/$N66</f>
+        <f t="shared" ref="V66:V78" si="38">I66/$N66</f>
         <v>0.23145232733426532</v>
       </c>
       <c r="W66">
-        <f t="shared" ref="W66:W79" si="39">J66/$N66</f>
+        <f t="shared" ref="W66:W78" si="39">J66/$N66</f>
         <v>0.23158950835993047</v>
       </c>
       <c r="X66">
-        <f t="shared" ref="X66:X79" si="40">K66/$N66</f>
+        <f t="shared" ref="X66:X78" si="40">K66/$N66</f>
         <v>0.11408335632441258</v>
       </c>
       <c r="Y66">
-        <f t="shared" ref="Y66:Y79" si="41">L66/$N66</f>
+        <f t="shared" ref="Y66:Y78" si="41">L66/$N66</f>
         <v>0.23133901408545579</v>
       </c>
       <c r="Z66" s="6">
-        <f t="shared" ref="Z66:Z97" si="42">(O66-$O$78)^2+(P66-$P$78)^2+(Q66-$Q$78)^2+(R66-$R$78)^2+(S66-$S$78)^2+(T66-$T$78)^2+(U66-$U$78)^2+(V66-$V$78)^2+(W66-$W$78)^2+(X66-$X$78)^2+(Y66-$Y$78)^2</f>
+        <f t="shared" ref="Z66:Z77" si="42">(O66-$O$78)^2+(P66-$P$78)^2+(Q66-$Q$78)^2+(R66-$R$78)^2+(S66-$S$78)^2+(T66-$T$78)^2+(U66-$U$78)^2+(V66-$V$78)^2+(W66-$W$78)^2+(X66-$X$78)^2+(Y66-$Y$78)^2</f>
         <v>0.11554591111236399</v>
       </c>
       <c r="AA66">
@@ -27292,7 +27295,7 @@
         <v>1.7814169037331747E-8</v>
       </c>
       <c r="C79" s="5">
-        <f t="shared" ref="C79:M79" si="45">1/C78</f>
+        <f t="shared" ref="C79:L79" si="45">1/C78</f>
         <v>6.291122314201925E-8</v>
       </c>
       <c r="D79" s="5">
@@ -27344,7 +27347,7 @@
         <v>8.1710624390757589E-2</v>
       </c>
       <c r="P79" s="5">
-        <f t="shared" ref="P79:AA79" si="46">C79/$N$79</f>
+        <f t="shared" ref="P79:Y79" si="46">C79/$N$79</f>
         <v>0.28856329550640841</v>
       </c>
       <c r="Q79" s="5">
@@ -27405,881 +27408,644 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>146</v>
       </c>
       <c r="B1" t="s">
         <v>894</v>
       </c>
-      <c r="C1" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>1.2863641711634177</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>208</v>
       </c>
       <c r="B3" s="5">
         <v>1.983501785968594E-2</v>
       </c>
-      <c r="C3">
-        <v>1.2422487049392812</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>235</v>
       </c>
       <c r="B4" s="5">
         <v>3.8742449168647948E-2</v>
       </c>
-      <c r="C4">
-        <v>1.1927097895907395</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>234</v>
       </c>
       <c r="B5" s="5">
         <v>4.6219255714104304E-2</v>
       </c>
-      <c r="C5">
-        <v>1.1633524877673711</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>209</v>
       </c>
       <c r="B6" s="5">
         <v>5.8495850301375829E-2</v>
       </c>
-      <c r="C6">
-        <v>1.2390376198285558</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>247</v>
       </c>
       <c r="B7" s="5">
         <v>6.1868156611234147E-2</v>
       </c>
-      <c r="C7">
-        <v>1.21342585649921</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B8" s="5">
         <v>7.687464269040449E-2</v>
       </c>
-      <c r="C8">
-        <v>1.1581040560968465</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>210</v>
       </c>
       <c r="B9" s="5">
         <v>8.4616982336195218E-2</v>
       </c>
-      <c r="C9">
-        <v>1.2910687499510245</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>213</v>
       </c>
       <c r="B10" s="5">
         <v>8.4616982336195218E-2</v>
       </c>
-      <c r="C10">
-        <v>1.2910687499510245</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>242</v>
       </c>
       <c r="B11" s="5">
         <v>8.4983521775686452E-2</v>
       </c>
-      <c r="C11">
-        <v>1.2837755807596425</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>153</v>
       </c>
       <c r="B12">
         <v>0.1025391989421116</v>
       </c>
-      <c r="C12">
-        <v>1.8442933523371126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>244</v>
       </c>
       <c r="B13">
         <v>0.11440112530454201</v>
       </c>
-      <c r="C13">
-        <v>1.0690556064497925</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>193</v>
       </c>
       <c r="B14">
         <v>0.11554591111236399</v>
       </c>
-      <c r="C14">
-        <v>0.813348275676125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>196</v>
       </c>
       <c r="B15">
         <v>0.12509756515455245</v>
       </c>
-      <c r="C15">
-        <v>0.76595401043350353</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>254</v>
       </c>
       <c r="B16">
         <v>0.1252280823423752</v>
       </c>
-      <c r="C16">
-        <v>0.76598361238882851</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>194</v>
       </c>
       <c r="B17">
         <v>0.14980735149345628</v>
       </c>
-      <c r="C17">
-        <v>0.68387506445253132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>186</v>
       </c>
       <c r="B18">
         <v>0.16481581099305556</v>
       </c>
-      <c r="C18">
-        <v>1.3054055402476969</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>248</v>
       </c>
       <c r="B19">
         <v>0.18795686537018105</v>
       </c>
-      <c r="C19">
-        <v>0.95107884432345158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>187</v>
       </c>
       <c r="B20">
         <v>0.23180464735346615</v>
       </c>
-      <c r="C20">
-        <v>0.86491794338260053</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>258</v>
       </c>
       <c r="B21">
         <v>0.23946002311876172</v>
       </c>
-      <c r="C21">
-        <v>0.7272719359837837</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>195</v>
       </c>
       <c r="B22">
         <v>0.24178820694343439</v>
       </c>
-      <c r="C22">
-        <v>1.3135956712269148</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>255</v>
       </c>
       <c r="B23">
         <v>0.24607981465305698</v>
       </c>
-      <c r="C23">
-        <v>0.90058354650718009</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>206</v>
       </c>
       <c r="B24">
         <v>0.25776297688791316</v>
       </c>
-      <c r="C24">
-        <v>0.69051852564540983</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>164</v>
       </c>
       <c r="B25">
         <v>0.27164040871641348</v>
       </c>
-      <c r="C25">
-        <v>1.9113905694071596</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>246</v>
       </c>
       <c r="B26">
         <v>0.2802849024133412</v>
       </c>
-      <c r="C26">
-        <v>0.78544909365758153</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>207</v>
       </c>
       <c r="B27">
         <v>0.29480535169364619</v>
       </c>
-      <c r="C27">
-        <v>0.69413872830333101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>189</v>
       </c>
       <c r="B28">
         <v>0.36694389153307044</v>
       </c>
-      <c r="C28">
-        <v>0.35849555801972666</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>260</v>
       </c>
       <c r="B29">
         <v>0.45303915198480443</v>
       </c>
-      <c r="C29">
-        <v>0.28651193117145834</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>192</v>
       </c>
       <c r="B30">
         <v>0.4835841957617415</v>
       </c>
-      <c r="C30">
-        <v>0.53514040563870335</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>265</v>
       </c>
       <c r="B31">
         <v>0.48881205187410987</v>
       </c>
-      <c r="C31">
-        <v>0.50596731846633336</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>178</v>
       </c>
       <c r="B32">
         <v>0.49124144002236947</v>
       </c>
-      <c r="C32">
-        <v>0.46796866713913243</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>266</v>
       </c>
       <c r="B33">
         <v>0.49950123957420306</v>
       </c>
-      <c r="C33">
-        <v>0.42216362021557663</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>171</v>
       </c>
       <c r="B34">
         <v>0.50604278476427278</v>
       </c>
-      <c r="C34">
-        <v>0.66837268420205997</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>245</v>
       </c>
       <c r="B35">
         <v>0.52630181842047952</v>
       </c>
-      <c r="C35">
-        <v>1.1810849816872619</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>191</v>
       </c>
       <c r="B36">
         <v>0.54598901056615801</v>
       </c>
-      <c r="C36">
-        <v>0.6413018663418415</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>168</v>
       </c>
       <c r="B37">
         <v>0.60817440937836009</v>
       </c>
-      <c r="C37">
-        <v>1.2518991550253544</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>151</v>
       </c>
       <c r="B38">
         <v>0.67228328738227416</v>
       </c>
-      <c r="C38">
-        <v>0.1734558268455855</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>205</v>
       </c>
       <c r="B39">
         <v>0.67636635745721563</v>
       </c>
-      <c r="C39">
-        <v>0.17092357313699114</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>149</v>
       </c>
       <c r="B40">
         <v>0.67641597599552084</v>
       </c>
-      <c r="C40">
-        <v>0.17142925132632592</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>154</v>
       </c>
       <c r="B41">
         <v>0.67641597599552084</v>
       </c>
-      <c r="C41">
-        <v>0.17142925132632592</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>175</v>
       </c>
       <c r="B42">
         <v>0.67748825489766895</v>
       </c>
-      <c r="C42">
-        <v>0.17082482540043609</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>201</v>
       </c>
       <c r="B43">
         <v>0.71615789906644478</v>
       </c>
-      <c r="C43">
-        <v>0.36525567574784396</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>262</v>
       </c>
       <c r="B44">
         <v>0.7908861178044414</v>
       </c>
-      <c r="C44">
-        <v>0.14359988007196522</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>253</v>
       </c>
       <c r="B45">
         <v>0.79563066510992386</v>
       </c>
-      <c r="C45">
-        <v>1.7600200434188495</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>156</v>
       </c>
       <c r="B46">
         <v>0.82834581072613356</v>
       </c>
-      <c r="C46">
-        <v>1.0471369341062429</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>157</v>
       </c>
       <c r="B47">
         <v>0.83584135151403938</v>
       </c>
-      <c r="C47">
-        <v>0.18258160055686615</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>179</v>
       </c>
       <c r="B48">
         <v>0.8374090661442859</v>
       </c>
-      <c r="C48">
-        <v>0.18923705688811968</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>199</v>
       </c>
       <c r="B49">
         <v>0.85797685912524502</v>
       </c>
-      <c r="C49">
-        <v>0.14944320570259181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>167</v>
       </c>
       <c r="B50">
         <v>0.86002885993450029</v>
       </c>
-      <c r="C50">
-        <v>0.13473608675756654</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
         <v>183</v>
       </c>
       <c r="B51" s="10">
         <v>0.86231094141308084</v>
       </c>
-      <c r="C51" s="10">
-        <v>0.13386664850869542</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>182</v>
       </c>
       <c r="B52" s="10">
         <v>0.86401411330049627</v>
       </c>
-      <c r="C52" s="10">
-        <v>0.13322322844865597</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>177</v>
       </c>
       <c r="B53">
         <v>0.87240804721357912</v>
       </c>
-      <c r="C53">
-        <v>0.21089632287789481</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>185</v>
       </c>
       <c r="B54" s="10">
         <v>0.89921091557767174</v>
       </c>
-      <c r="C54" s="10">
-        <v>0.11683866780392574</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>184</v>
       </c>
       <c r="B55">
         <v>0.91003420042885952</v>
       </c>
-      <c r="C55">
-        <v>0.96402524281225399</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>150</v>
       </c>
       <c r="B56">
         <v>0.91026324557430849</v>
       </c>
-      <c r="C56">
-        <v>0.2249811381715999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>155</v>
       </c>
       <c r="B57">
         <v>0.91026324557430849</v>
       </c>
-      <c r="C57">
-        <v>0.2249811381715999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>264</v>
       </c>
       <c r="B58">
         <v>0.94908777644584441</v>
       </c>
-      <c r="C58">
-        <v>1.3039124897959502</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>165</v>
       </c>
       <c r="B59">
         <v>0.97978664848469799</v>
       </c>
-      <c r="C59">
-        <v>1.5293891483218662</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>172</v>
       </c>
       <c r="B60">
         <v>0.97978664848469799</v>
       </c>
-      <c r="C60">
-        <v>1.5293891483218662</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
         <v>162</v>
       </c>
       <c r="B61" s="10">
         <v>1.0512552016256058</v>
       </c>
-      <c r="C61" s="10">
-        <v>7.8011749496288765E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>188</v>
       </c>
       <c r="B62">
         <v>1.0537934507891407</v>
       </c>
-      <c r="C62">
-        <v>1.7874752674642231</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>152</v>
       </c>
       <c r="B63">
         <v>1.0799674543502225</v>
       </c>
-      <c r="C63">
-        <v>1.6758204690056842</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
         <v>200</v>
       </c>
       <c r="B64" s="10">
         <v>1.0976228119176703</v>
       </c>
-      <c r="C64" s="10">
-        <v>8.660305668560582E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
         <v>256</v>
       </c>
       <c r="B65" s="10">
         <v>1.1086252284276503</v>
       </c>
-      <c r="C65" s="10">
-        <v>1.1612596896463824E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>173</v>
       </c>
       <c r="B66">
         <v>1.1117419028711597</v>
       </c>
-      <c r="C66">
-        <v>0.19400578863682469</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
         <v>163</v>
       </c>
       <c r="B67" s="10">
         <v>1.1217879229966849</v>
       </c>
-      <c r="C67" s="10">
-        <v>1.0393380290139611E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>158</v>
       </c>
       <c r="B68">
         <v>1.1676847065379115</v>
       </c>
-      <c r="C68">
-        <v>1.6415372052940189</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>218</v>
       </c>
       <c r="B69">
         <v>1.1769079552365933</v>
       </c>
-      <c r="C69">
-        <v>1.1144135092776197</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>259</v>
       </c>
       <c r="B70">
         <v>1.1817484835008534</v>
       </c>
-      <c r="C70">
-        <v>0.20735476022491223</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>202</v>
       </c>
       <c r="B71">
         <v>1.1958181287757219</v>
       </c>
-      <c r="C71">
-        <v>1.8120762961148571</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>161</v>
       </c>
       <c r="B72">
         <v>1.2370507757884783</v>
       </c>
-      <c r="C72">
-        <v>0.18221191004009044</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>204</v>
       </c>
       <c r="B73">
         <v>1.2738482354913316</v>
       </c>
-      <c r="C73">
-        <v>0.40178323880130851</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
         <v>160</v>
       </c>
       <c r="B74" s="10">
         <v>1.2832287183511688</v>
       </c>
-      <c r="C74" s="10">
-        <v>5.6356696078252541E-2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>892</v>
       </c>
       <c r="B75">
         <v>1.2863641711634177</v>
       </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>170</v>
       </c>
       <c r="B76">
         <v>1.3420822202321552</v>
       </c>
-      <c r="C76">
-        <v>0.98097387489384424</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>239</v>
       </c>
       <c r="B77">
         <v>1.7026276120426931</v>
       </c>
-      <c r="C77">
-        <v>1.1272540289643045</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>176</v>
       </c>
       <c r="B78">
         <v>1.7026276122011084</v>
       </c>
-      <c r="C78">
-        <v>1.1272540289537216</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>236</v>
       </c>
       <c r="B79">
         <v>2</v>
-      </c>
-      <c r="C79">
-        <v>1.1272539078086741</v>
       </c>
     </row>
   </sheetData>
@@ -28295,7 +28061,7 @@
   <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28313,7 +28079,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
       <c r="B2">
         <v>0</v>

</xml_diff>